<commit_message>
vul data aan met werkzaamheidsgraad
</commit_message>
<xml_diff>
--- a/dynam_jobevolution/20180425_dynam_be_jobdata_origineel.xlsx
+++ b/dynam_jobevolution/20180425_dynam_be_jobdata_origineel.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>bruto toename</t>
   </si>
@@ -85,12 +85,18 @@
   </si>
   <si>
     <t>02000</t>
+  </si>
+  <si>
+    <t>werkzaamheidsgraad_2016</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,13 +134,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,10 +545,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,7 +556,7 @@
     <col min="1" max="1" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -568,8 +575,11 @@
       <c r="J1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -597,8 +607,11 @@
       <c r="J2" s="1">
         <v>1.0516946572037569E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L2" s="4">
+        <v>69.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -626,8 +639,11 @@
       <c r="J3" s="1">
         <v>1.1994191776310698E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L3" s="4">
+        <v>59.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -655,8 +671,11 @@
       <c r="J4" s="1">
         <v>1.1363573920927551E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L4" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -684,8 +703,11 @@
       <c r="J5" s="1">
         <v>1.9719771665801772E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L5" s="4">
+        <v>69.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -713,8 +735,11 @@
       <c r="J6" s="1">
         <v>1.4801546001663342E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L6" s="4">
+        <v>61.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -742,8 +767,11 @@
       <c r="J7" s="1">
         <v>2.0416317587162468E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L7" s="4">
+        <v>68.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -771,8 +799,11 @@
       <c r="J8" s="1">
         <v>2.1202034516472769E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L8" s="4">
+        <v>64.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -800,8 +831,11 @@
       <c r="J9" s="1">
         <v>1.6573923570675775E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L9" s="4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -829,8 +863,11 @@
       <c r="J10" s="1">
         <v>1.4154341193690918E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L10" s="4">
+        <v>73.900000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -858,8 +895,11 @@
       <c r="J11" s="1">
         <v>1.8153627751495954E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L11" s="4">
+        <v>69.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -887,8 +927,12 @@
       <c r="J12" s="1">
         <v>1.5461061981844437E-2</v>
       </c>
+      <c r="L12" s="4">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>